<commit_message>
Add pit-scouting data for each team from the Google Form and export it to Firebase/Excel
</commit_message>
<xml_diff>
--- a/paly_from_8th.xlsx
+++ b/paly_from_8th.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14160" windowWidth="21860" xWindow="60" yWindow="1120"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14160" windowWidth="21860" xWindow="60" yWindow="1120"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Export" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,9 +24,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="0\%" numFmtId="164"/>
-    <numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" numFmtId="165"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -240,8 +239,11 @@
     <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -256,11 +258,8 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3877,48 +3876,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>868</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -3931,7 +3930,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -3948,7 +3947,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -3965,7 +3964,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -3988,7 +3987,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -4000,7 +3999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -4035,7 +4034,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -4047,7 +4046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -4077,7 +4076,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -4089,7 +4088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -4119,9 +4118,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -4131,7 +4128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -4165,7 +4162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -4199,7 +4196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -4211,7 +4208,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -4232,7 +4229,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -4245,6 +4242,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Mecanum</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -4271,14 +4274,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -4300,7 +4295,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -4315,11 +4310,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>7</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -4342,7 +4337,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -4355,6 +4350,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>7</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -4376,7 +4379,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -4461,7 +4464,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -4480,8 +4483,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -4489,12 +4492,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -4502,12 +4505,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -4515,12 +4518,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -4722,7 +4725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -4982,7 +4985,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -5001,7 +5004,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -5825,7 +5828,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -5835,6 +5838,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -5849,51 +5853,51 @@
   <dimension ref="A1:CY39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="n">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="n">
         <v>1114</v>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -5923,7 +5927,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>10</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -5963,7 +5967,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -5975,7 +5979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -6010,7 +6014,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>90</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -6022,7 +6026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -6052,7 +6056,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -6064,7 +6068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -6094,7 +6098,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
+      <c r="K8" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="2" t="inlineStr">
@@ -6106,7 +6110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -6140,7 +6144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -6174,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -6186,7 +6190,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -6207,7 +6211,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -6220,6 +6224,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Swerve</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -6246,14 +6256,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>15</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -6275,7 +6277,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>85</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -6290,11 +6292,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>4</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -6317,7 +6319,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>15</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -6330,6 +6332,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>4</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -6351,7 +6361,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>95</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -6436,7 +6446,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -6455,8 +6465,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -6464,12 +6474,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -6477,12 +6487,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -6490,12 +6500,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -6697,7 +6707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -6957,7 +6967,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -6976,7 +6986,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -7800,7 +7810,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -7810,6 +7820,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B12">
     <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
@@ -7839,48 +7850,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>1114</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -7893,7 +7904,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -7910,7 +7921,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -7927,7 +7938,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -7950,7 +7961,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -7962,7 +7973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -7997,7 +8008,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -8009,7 +8020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -8039,7 +8050,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -8051,7 +8062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -8081,9 +8092,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -8093,7 +8102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -8127,7 +8136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -8161,7 +8170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -8173,7 +8182,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -8194,7 +8203,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -8207,6 +8216,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Tank</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -8233,14 +8248,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -8262,7 +8269,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -8277,11 +8284,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>7</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -8304,7 +8311,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -8317,6 +8324,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>7</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -8338,7 +8353,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -8423,7 +8438,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -8442,8 +8457,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -8451,12 +8466,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -8464,12 +8479,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -8477,12 +8492,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -8684,7 +8699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -8944,7 +8959,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -8963,7 +8978,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -9787,7 +9802,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -9797,6 +9812,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -9816,48 +9832,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>2337</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -9870,7 +9886,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -9887,7 +9903,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -9904,7 +9920,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -9927,7 +9943,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -9939,7 +9955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -9974,7 +9990,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -9986,7 +10002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -10016,7 +10032,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -10028,7 +10044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -10058,9 +10074,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -10070,7 +10084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -10104,7 +10118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -10138,7 +10152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -10150,7 +10164,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -10171,7 +10185,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -10184,6 +10198,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Tank Treads</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -10210,14 +10230,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>8</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -10239,7 +10251,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -10254,11 +10266,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>49</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -10281,7 +10293,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -10294,6 +10306,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>49</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -10315,7 +10335,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -10400,7 +10420,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -10419,8 +10439,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -10428,12 +10448,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -10441,12 +10461,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -10454,12 +10474,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -10661,7 +10681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -10921,7 +10941,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -10940,7 +10960,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -11764,7 +11784,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -11774,6 +11794,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -11793,48 +11814,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>3044</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -11847,7 +11868,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -11864,7 +11885,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -11881,7 +11902,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -11904,7 +11925,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -11916,7 +11937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -11951,7 +11972,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -11963,7 +11984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -11993,7 +12014,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n"/>
+      <c r="K7" s="16" t="n"/>
       <c r="M7" s="2" t="inlineStr">
         <is>
           <t>Rocket</t>
@@ -12003,7 +12024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -12033,8 +12054,8 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
+      <c r="K8" s="16" t="n">
+        <v>100</v>
       </c>
       <c r="M8" s="2" t="inlineStr">
         <is>
@@ -12045,7 +12066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -12079,7 +12100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -12113,7 +12134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -12125,7 +12146,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -12146,7 +12167,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -12159,6 +12180,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Slide</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -12185,14 +12212,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -12214,7 +12233,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -12229,11 +12248,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>9</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -12256,7 +12275,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -12269,6 +12288,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>9</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -12290,7 +12317,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -12375,7 +12402,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -12394,8 +12421,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -12403,12 +12430,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -12416,12 +12443,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -12429,12 +12456,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -12636,7 +12663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -12896,7 +12923,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -12915,7 +12942,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -13739,7 +13766,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -13749,6 +13776,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -13768,48 +13796,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>3381</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -13822,7 +13850,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -13839,7 +13867,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -13856,7 +13884,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -13879,7 +13907,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -13891,7 +13919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -13926,7 +13954,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -13938,7 +13966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -13968,7 +13996,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n"/>
+      <c r="K7" s="16" t="n"/>
       <c r="M7" s="2" t="inlineStr">
         <is>
           <t>Rocket</t>
@@ -13978,7 +14006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -14008,9 +14036,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -14020,7 +14046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -14054,7 +14080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -14088,7 +14114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -14100,7 +14126,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -14121,7 +14147,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -14134,6 +14160,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -14160,14 +14192,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -14189,7 +14213,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -14204,11 +14228,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>2</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -14231,7 +14255,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -14244,6 +14268,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>2</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -14265,7 +14297,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -14350,7 +14382,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -14369,8 +14401,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -14378,12 +14410,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -14391,12 +14423,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -14404,12 +14436,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -14611,7 +14643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -14871,7 +14903,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -14890,7 +14922,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -15714,7 +15746,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -15724,6 +15756,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -15743,48 +15776,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>4381</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -15797,7 +15830,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -15814,7 +15847,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -15831,7 +15864,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -15854,7 +15887,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -15866,7 +15899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -15901,7 +15934,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -15913,7 +15946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -15943,7 +15976,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -15955,7 +15988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -15985,9 +16018,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -15997,7 +16028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -16031,7 +16062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -16065,7 +16096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -16077,7 +16108,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -16098,7 +16129,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -16111,6 +16142,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>H Drive</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -16137,14 +16174,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -16166,7 +16195,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -16181,11 +16210,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>38</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -16208,7 +16237,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -16221,6 +16250,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>38</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -16242,7 +16279,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -16327,7 +16364,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -16346,8 +16383,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -16355,12 +16392,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -16368,12 +16405,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -16381,12 +16418,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -16588,7 +16625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -16848,7 +16885,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -16867,7 +16904,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -17691,7 +17728,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -17701,6 +17738,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -17720,48 +17758,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>51</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -17774,7 +17812,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -17791,7 +17829,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -17808,7 +17846,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -17831,7 +17869,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -17843,7 +17881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -17878,7 +17916,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -17890,7 +17928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -17920,7 +17958,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M7" s="2" t="inlineStr">
@@ -17932,7 +17970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -17962,9 +18000,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -17974,7 +18010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -18008,7 +18044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -18042,7 +18078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -18054,7 +18090,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -18075,7 +18111,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -18088,6 +18124,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Swerve</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -18114,14 +18156,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -18143,7 +18177,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -18158,11 +18192,11 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Avg Time Climbing</t>
-        </is>
-      </c>
-      <c r="B15" s="25" t="n">
-        <v>38</v>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
@@ -18185,7 +18219,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -18198,6 +18232,14 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Avg Time Climbing</t>
+        </is>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>38</v>
+      </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -18219,7 +18261,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -18304,7 +18346,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -18323,8 +18365,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -18332,12 +18374,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -18345,12 +18387,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -18358,12 +18400,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -18565,7 +18607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -18825,7 +18867,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -18844,7 +18886,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -19668,7 +19710,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -19678,6 +19720,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -19697,48 +19740,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="18" width="15"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="7"/>
-    <col customWidth="1" max="3" min="3" style="18" width="6.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="15.1640625"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6"/>
-    <col customWidth="1" max="6" min="6" style="18" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="12.83203125"/>
-    <col customWidth="1" max="8" min="8" style="18" width="6.5"/>
-    <col customWidth="1" max="9" min="9" style="18" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="18" width="16"/>
-    <col customWidth="1" max="13" min="13" style="18" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="15"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="19" width="7"/>
+    <col customWidth="1" max="3" min="3" style="19" width="6.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="19" width="15.1640625"/>
+    <col customWidth="1" max="5" min="5" style="19" width="6"/>
+    <col customWidth="1" max="6" min="6" style="19" width="7.5"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="19" width="12.83203125"/>
+    <col customWidth="1" max="8" min="8" style="19" width="6.5"/>
+    <col customWidth="1" max="9" min="9" style="19" width="7.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="19" width="16"/>
+    <col customWidth="1" max="13" min="13" style="19" width="15.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="18">
-      <c r="A1" s="22" t="inlineStr">
+    <row customHeight="1" ht="24" r="1" s="19">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>7651</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="2" s="18">
+    <row customHeight="1" ht="20" r="2" s="19">
       <c r="A2" s="15" t="inlineStr">
         <is>
-          <t>Simbotics - St Catharines</t>
-        </is>
-      </c>
-      <c r="D2" s="23" t="inlineStr">
+          <t>Simbotics</t>
+        </is>
+      </c>
+      <c r="D2" s="24" t="inlineStr">
         <is>
           <t>Cycle Times</t>
         </is>
       </c>
-      <c r="G2" s="23" t="inlineStr">
+      <c r="G2" s="24" t="inlineStr">
         <is>
           <t>Teleop Cycle Totals</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="24" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="M2" s="23" t="inlineStr">
+      <c r="M2" s="24" t="inlineStr">
         <is>
           <t>Last Three Matches</t>
         </is>
@@ -19751,7 +19794,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -19768,7 +19811,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -19785,7 +19828,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -19808,7 +19851,7 @@
           <t>Level 2 %</t>
         </is>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
@@ -19820,7 +19863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="6" s="18">
+    <row customHeight="1" ht="16" r="6" s="19">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Level 2</t>
@@ -19855,7 +19898,7 @@
           <t>Level 3 %</t>
         </is>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="inlineStr">
@@ -19867,7 +19910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="7" s="18">
+    <row customHeight="1" ht="16" r="7" s="19">
       <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Level 3</t>
@@ -19897,7 +19940,7 @@
           <t>Level 3 Success Rate</t>
         </is>
       </c>
-      <c r="K7" s="17" t="n"/>
+      <c r="K7" s="16" t="n"/>
       <c r="M7" s="2" t="inlineStr">
         <is>
           <t>Rocket</t>
@@ -19907,7 +19950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="8" s="18">
+    <row customHeight="1" ht="16" r="8" s="19">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Can Start Hab 2</t>
@@ -19937,9 +19980,7 @@
           <t>Level 2 Success Rate</t>
         </is>
       </c>
-      <c r="K8" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K8" s="16" t="n"/>
       <c r="M8" s="2" t="inlineStr">
         <is>
           <t>Cargo Ship</t>
@@ -19949,7 +19990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="9" s="18">
+    <row customHeight="1" ht="16" r="9" s="19">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Climb Level 2</t>
@@ -19983,7 +20024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="10" s="18">
+    <row customHeight="1" ht="16" r="10" s="19">
       <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Climb Level 3</t>
@@ -20017,7 +20058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="11" s="18">
+    <row customHeight="1" ht="16" r="11" s="19">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cargo</t>
@@ -20029,7 +20070,7 @@
       <c r="E11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="12" s="18">
+    <row customHeight="1" ht="16" r="12" s="19">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Hatch</t>
@@ -20050,7 +20091,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n"/>
-      <c r="J12" s="19" t="inlineStr">
+      <c r="J12" s="20" t="inlineStr">
         <is>
           <t>Sandstorm</t>
         </is>
@@ -20063,6 +20104,12 @@
       <c r="N12" s="3" t="n"/>
     </row>
     <row r="13">
+      <c r="A13" s="25" t="inlineStr">
+        <is>
+          <t>Swerve</t>
+        </is>
+      </c>
+      <c r="B13" s="22" t="n"/>
       <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Hatch Level 1</t>
@@ -20089,14 +20136,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>% Defense</t>
-        </is>
-      </c>
-      <c r="B14" s="17" t="n">
-        <v>75</v>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Cargo Level 1</t>
@@ -20118,7 +20157,7 @@
           <t>Level 1 %</t>
         </is>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -20133,46 +20172,54 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
+          <t>% Defense</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Hatch Undefended</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Rocket</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>Level 2 %</t>
+        </is>
+      </c>
+      <c r="K15" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="inlineStr">
+        <is>
+          <t>Hatch Undefended</t>
+        </is>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
           <t>Avg Time Climbing</t>
         </is>
       </c>
-      <c r="B15" s="25" t="n">
+      <c r="B16" s="18" t="n">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>Hatch Undefended</t>
-        </is>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="inlineStr">
-        <is>
-          <t>Rocket</t>
-        </is>
-      </c>
-      <c r="H15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>Level 2 %</t>
-        </is>
-      </c>
-      <c r="K15" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2" t="inlineStr">
-        <is>
-          <t>Hatch Undefended</t>
-        </is>
-      </c>
-      <c r="N15" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
       <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Hatch Defended</t>
@@ -20194,7 +20241,7 @@
           <t>Leave Hab %</t>
         </is>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="16" t="n">
         <v>100</v>
       </c>
       <c r="M16" s="2" t="inlineStr">
@@ -20279,7 +20326,7 @@
       <c r="H19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="20" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="20" s="19" thickBot="1">
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="6" t="n"/>
@@ -20298,8 +20345,8 @@
       <c r="P20" s="6" t="n"/>
       <c r="Q20" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="21" s="18" thickTop="1"/>
-    <row customHeight="1" ht="19" r="22" s="18">
+    <row customHeight="1" ht="16" r="21" s="19" thickTop="1"/>
+    <row customHeight="1" ht="19" r="22" s="19">
       <c r="A22" s="8" t="inlineStr">
         <is>
           <t>QM 112</t>
@@ -20307,12 +20354,12 @@
       </c>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="D22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="E22" s="21" t="n"/>
+      <c r="E22" s="22" t="n"/>
       <c r="G22" s="8" t="inlineStr">
         <is>
           <t>QM 27</t>
@@ -20320,12 +20367,12 @@
       </c>
       <c r="H22" s="9" t="n"/>
       <c r="I22" s="9" t="n"/>
-      <c r="J22" s="20" t="inlineStr">
+      <c r="J22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="K22" s="21" t="n"/>
+      <c r="K22" s="22" t="n"/>
       <c r="M22" s="8" t="inlineStr">
         <is>
           <t>QM 4</t>
@@ -20333,12 +20380,12 @@
       </c>
       <c r="N22" s="9" t="n"/>
       <c r="O22" s="9" t="n"/>
-      <c r="P22" s="20" t="inlineStr">
+      <c r="P22" s="21" t="inlineStr">
         <is>
           <t>Cycles Done</t>
         </is>
       </c>
-      <c r="Q22" s="21" t="n"/>
+      <c r="Q22" s="22" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -20540,7 +20587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="27" s="18">
+    <row customHeight="1" ht="16" r="27" s="19">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Left Hab</t>
@@ -20800,7 +20847,7 @@
       <c r="P33" s="12" t="n"/>
       <c r="Q33" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="36" s="18" thickBot="1">
+    <row customHeight="1" ht="16" r="36" s="19" thickBot="1">
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="6" t="n"/>
       <c r="C36" s="6" t="n"/>
@@ -20819,7 +20866,7 @@
       <c r="P36" s="6" t="n"/>
       <c r="Q36" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="16" r="37" s="18" thickTop="1">
+    <row customHeight="1" ht="16" r="37" s="19" thickTop="1">
       <c r="E37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="K37" s="3" t="n"/>
@@ -21643,7 +21690,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J22:K22"/>
@@ -21653,6 +21700,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>